<commit_message>
update the attribute datasets
</commit_message>
<xml_diff>
--- a/arvarto-customer-segmentation/data-dictionary/DIAS Information Levels - Attributes 2017.xlsx
+++ b/arvarto-customer-segmentation/data-dictionary/DIAS Information Levels - Attributes 2017.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Merkmalskatalog\Merkmale englisch\Neue Dateien\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bfernandes\Documents\repositories\portfolio\arvarto-customer-segmentation\data-dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9D8BF1-5198-49C4-96EB-69E96B31E684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396"/>
+    <workbookView xWindow="-83" yWindow="-83" windowWidth="25966" windowHeight="10366" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Komplett" sheetId="1" r:id="rId1"/>
@@ -1975,7 +1976,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2365,7 +2366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2488,8 +2489,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2533,7 +2532,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2542,68 +2541,68 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2623,9 +2622,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2663,9 +2662,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2700,7 +2699,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2735,7 +2734,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2908,31 +2907,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:E315"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C185" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D64" sqref="D64"/>
+      <selection pane="bottomRight" activeCell="D191" sqref="D191"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.46484375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="4.1328125" style="2" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="11.44140625" style="2"/>
+    <col min="3" max="3" width="39.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.46484375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.86328125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="11.46484375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:5" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:5" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>131</v>
       </c>
@@ -2946,7 +2945,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="51" x14ac:dyDescent="0.35">
       <c r="B3" s="41"/>
       <c r="C3" s="34" t="s">
         <v>110</v>
@@ -2958,8 +2957,8 @@
         <v>646</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="B4" s="80" t="s">
+    <row r="4" spans="2:5" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="B4" s="75" t="s">
         <v>348</v>
       </c>
       <c r="C4" s="34" t="s">
@@ -2968,12 +2967,12 @@
       <c r="D4" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="E4" s="63" t="s">
+      <c r="E4" s="61" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B5" s="80"/>
+    <row r="5" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B5" s="75"/>
       <c r="C5" s="6" t="s">
         <v>18</v>
       </c>
@@ -2982,92 +2981,92 @@
       </c>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="2:5" ht="145.19999999999999" x14ac:dyDescent="0.25">
-      <c r="B6" s="80"/>
+    <row r="6" spans="2:5" ht="140.25" x14ac:dyDescent="0.35">
+      <c r="B6" s="75"/>
       <c r="C6" s="34" t="s">
         <v>316</v>
       </c>
-      <c r="D6" s="55" t="s">
+      <c r="D6" s="53" t="s">
         <v>416</v>
       </c>
-      <c r="E6" s="63" t="s">
+      <c r="E6" s="61" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B7" s="80"/>
+    <row r="7" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B7" s="75"/>
       <c r="C7" s="18" t="s">
         <v>114</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="E7" s="76" t="s">
+      <c r="E7" s="70" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B8" s="80"/>
+    <row r="8" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B8" s="75"/>
       <c r="C8" s="18" t="s">
         <v>115</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="E8" s="77"/>
-    </row>
-    <row r="9" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B9" s="80"/>
+      <c r="E8" s="71"/>
+    </row>
+    <row r="9" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B9" s="75"/>
       <c r="C9" s="18" t="s">
         <v>116</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="E9" s="77"/>
-    </row>
-    <row r="10" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B10" s="80"/>
+      <c r="E9" s="71"/>
+    </row>
+    <row r="10" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B10" s="75"/>
       <c r="C10" s="18" t="s">
         <v>117</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="E10" s="77"/>
-    </row>
-    <row r="11" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B11" s="80"/>
+      <c r="E10" s="71"/>
+    </row>
+    <row r="11" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B11" s="75"/>
       <c r="C11" s="18" t="s">
         <v>118</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="E11" s="77"/>
-    </row>
-    <row r="12" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B12" s="80"/>
+      <c r="E11" s="71"/>
+    </row>
+    <row r="12" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B12" s="75"/>
       <c r="C12" s="18" t="s">
         <v>119</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="E12" s="77"/>
-    </row>
-    <row r="13" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B13" s="80"/>
+      <c r="E12" s="71"/>
+    </row>
+    <row r="13" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B13" s="75"/>
       <c r="C13" s="18" t="s">
         <v>120</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="E13" s="77"/>
-    </row>
-    <row r="14" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="80"/>
+      <c r="E13" s="71"/>
+    </row>
+    <row r="14" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="75"/>
       <c r="C14" s="6" t="s">
         <v>22</v>
       </c>
@@ -3076,8 +3075,8 @@
       </c>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B15" s="80"/>
+    <row r="15" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B15" s="75"/>
       <c r="C15" s="18" t="s">
         <v>589</v>
       </c>
@@ -3086,20 +3085,20 @@
       </c>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="2:5" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="B16" s="80"/>
-      <c r="C16" s="53" t="s">
+    <row r="16" spans="2:5" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="B16" s="75"/>
+      <c r="C16" s="51" t="s">
         <v>352</v>
       </c>
-      <c r="D16" s="54" t="s">
+      <c r="D16" s="52" t="s">
         <v>417</v>
       </c>
-      <c r="E16" s="63" t="s">
+      <c r="E16" s="61" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="B17" s="80"/>
+    <row r="17" spans="2:5" ht="51" x14ac:dyDescent="0.35">
+      <c r="B17" s="75"/>
       <c r="C17" s="34" t="s">
         <v>107</v>
       </c>
@@ -3110,32 +3109,32 @@
         <v>646</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B18" s="80"/>
-      <c r="C18" s="64" t="s">
+    <row r="18" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B18" s="75"/>
+      <c r="C18" s="62" t="s">
         <v>568</v>
       </c>
-      <c r="D18" s="64" t="s">
+      <c r="D18" s="62" t="s">
         <v>422</v>
       </c>
-      <c r="E18" s="65" t="s">
+      <c r="E18" s="63" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B19" s="80"/>
-      <c r="C19" s="64" t="s">
+    <row r="19" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B19" s="75"/>
+      <c r="C19" s="62" t="s">
         <v>569</v>
       </c>
-      <c r="D19" s="64" t="s">
+      <c r="D19" s="62" t="s">
         <v>423</v>
       </c>
-      <c r="E19" s="65" t="s">
+      <c r="E19" s="63" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B20" s="80"/>
+    <row r="20" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B20" s="75"/>
       <c r="C20" s="18" t="s">
         <v>570</v>
       </c>
@@ -3144,8 +3143,8 @@
       </c>
       <c r="E20" s="12"/>
     </row>
-    <row r="21" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B21" s="80"/>
+    <row r="21" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B21" s="75"/>
       <c r="C21" s="18" t="s">
         <v>571</v>
       </c>
@@ -3154,8 +3153,8 @@
       </c>
       <c r="E21" s="12"/>
     </row>
-    <row r="22" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B22" s="80"/>
+    <row r="22" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B22" s="75"/>
       <c r="C22" s="18" t="s">
         <v>572</v>
       </c>
@@ -3164,8 +3163,8 @@
       </c>
       <c r="E22" s="12"/>
     </row>
-    <row r="23" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B23" s="80"/>
+    <row r="23" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B23" s="75"/>
       <c r="C23" s="18" t="s">
         <v>573</v>
       </c>
@@ -3174,32 +3173,32 @@
       </c>
       <c r="E23" s="12"/>
     </row>
-    <row r="24" spans="2:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B24" s="80"/>
+    <row r="24" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="75"/>
       <c r="C24" s="34" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="E24" s="63" t="s">
+      <c r="E24" s="61" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="B25" s="80"/>
-      <c r="C25" s="53" t="s">
+    <row r="25" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B25" s="75"/>
+      <c r="C25" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="D25" s="53" t="s">
+      <c r="D25" s="51" t="s">
         <v>246</v>
       </c>
-      <c r="E25" s="63" t="s">
+      <c r="E25" s="61" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B26" s="80"/>
+    <row r="26" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B26" s="75"/>
       <c r="C26" s="18" t="s">
         <v>587</v>
       </c>
@@ -3208,160 +3207,160 @@
       </c>
       <c r="E26" s="12"/>
     </row>
-    <row r="27" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B27" s="80"/>
+    <row r="27" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B27" s="75"/>
       <c r="C27" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="E27" s="83" t="s">
+      <c r="E27" s="81" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B28" s="80"/>
+    <row r="28" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B28" s="75"/>
       <c r="C28" s="6" t="s">
         <v>94</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="E28" s="84"/>
-    </row>
-    <row r="29" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B29" s="80"/>
+      <c r="E28" s="82"/>
+    </row>
+    <row r="29" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B29" s="75"/>
       <c r="C29" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="E29" s="84"/>
-    </row>
-    <row r="30" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B30" s="80"/>
+      <c r="E29" s="82"/>
+    </row>
+    <row r="30" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B30" s="75"/>
       <c r="C30" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="E30" s="84"/>
-    </row>
-    <row r="31" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B31" s="80"/>
+      <c r="E30" s="82"/>
+    </row>
+    <row r="31" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B31" s="75"/>
       <c r="C31" s="6" t="s">
         <v>97</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="E31" s="84"/>
-    </row>
-    <row r="32" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B32" s="80"/>
+      <c r="E31" s="82"/>
+    </row>
+    <row r="32" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B32" s="75"/>
       <c r="C32" s="6" t="s">
         <v>98</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="E32" s="84"/>
-    </row>
-    <row r="33" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B33" s="80"/>
+      <c r="E32" s="82"/>
+    </row>
+    <row r="33" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B33" s="75"/>
       <c r="C33" s="6" t="s">
         <v>99</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="E33" s="84"/>
-    </row>
-    <row r="34" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B34" s="80"/>
+      <c r="E33" s="82"/>
+    </row>
+    <row r="34" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B34" s="75"/>
       <c r="C34" s="6" t="s">
         <v>100</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="E34" s="84"/>
-    </row>
-    <row r="35" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B35" s="80"/>
+      <c r="E34" s="82"/>
+    </row>
+    <row r="35" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B35" s="75"/>
       <c r="C35" s="6" t="s">
         <v>101</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="E35" s="84"/>
-    </row>
-    <row r="36" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B36" s="80"/>
+      <c r="E35" s="82"/>
+    </row>
+    <row r="36" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B36" s="75"/>
       <c r="C36" s="6" t="s">
         <v>102</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="E36" s="84"/>
-    </row>
-    <row r="37" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B37" s="80"/>
+      <c r="E36" s="82"/>
+    </row>
+    <row r="37" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B37" s="75"/>
       <c r="C37" s="6" t="s">
         <v>103</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="E37" s="84"/>
-    </row>
-    <row r="38" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B38" s="80"/>
+      <c r="E37" s="82"/>
+    </row>
+    <row r="38" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B38" s="75"/>
       <c r="C38" s="6" t="s">
         <v>104</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="E38" s="84"/>
-    </row>
-    <row r="39" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B39" s="80"/>
+      <c r="E38" s="82"/>
+    </row>
+    <row r="39" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B39" s="75"/>
       <c r="C39" s="6" t="s">
         <v>105</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="E39" s="84"/>
-    </row>
-    <row r="40" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B40" s="80"/>
+      <c r="E39" s="82"/>
+    </row>
+    <row r="40" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B40" s="75"/>
       <c r="C40" s="6" t="s">
         <v>106</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="E40" s="84"/>
-    </row>
-    <row r="41" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B41" s="80"/>
+      <c r="E40" s="82"/>
+    </row>
+    <row r="41" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B41" s="75"/>
       <c r="C41" s="6" t="s">
         <v>108</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="E41" s="85"/>
-    </row>
-    <row r="42" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B42" s="80"/>
+      <c r="E41" s="83"/>
+    </row>
+    <row r="42" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B42" s="75"/>
       <c r="C42" s="6" t="s">
         <v>113</v>
       </c>
@@ -3370,8 +3369,8 @@
       </c>
       <c r="E42" s="46"/>
     </row>
-    <row r="43" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B43" s="80"/>
+    <row r="43" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B43" s="75"/>
       <c r="C43" s="22" t="s">
         <v>19</v>
       </c>
@@ -3380,32 +3379,32 @@
       </c>
       <c r="E43" s="26"/>
     </row>
-    <row r="44" spans="2:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B44" s="80"/>
-      <c r="C44" s="52" t="s">
+    <row r="44" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B44" s="75"/>
+      <c r="C44" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="D44" s="52" t="s">
+      <c r="D44" s="50" t="s">
         <v>237</v>
       </c>
       <c r="E44" s="45" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="45" spans="2:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="81"/>
-      <c r="C45" s="66" t="s">
+    <row r="45" spans="2:5" ht="25.9" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B45" s="76"/>
+      <c r="C45" s="64" t="s">
         <v>353</v>
       </c>
-      <c r="D45" s="67" t="s">
+      <c r="D45" s="65" t="s">
         <v>421</v>
       </c>
-      <c r="E45" s="68" t="s">
+      <c r="E45" s="66" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="46" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B46" s="73" t="s">
+    <row r="46" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B46" s="74" t="s">
         <v>347</v>
       </c>
       <c r="C46" s="21" t="s">
@@ -3416,8 +3415,8 @@
       </c>
       <c r="E46" s="4"/>
     </row>
-    <row r="47" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B47" s="73"/>
+    <row r="47" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B47" s="74"/>
       <c r="C47" s="5" t="s">
         <v>15</v>
       </c>
@@ -3426,8 +3425,8 @@
       </c>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B48" s="73"/>
+    <row r="48" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B48" s="74"/>
       <c r="C48" s="5" t="s">
         <v>16</v>
       </c>
@@ -3436,8 +3435,8 @@
       </c>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B49" s="73"/>
+    <row r="49" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B49" s="74"/>
       <c r="C49" s="5" t="s">
         <v>17</v>
       </c>
@@ -3446,292 +3445,292 @@
       </c>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="2:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B50" s="73"/>
-      <c r="C50" s="62" t="s">
+    <row r="50" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B50" s="74"/>
+      <c r="C50" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="D50" s="62" t="s">
+      <c r="D50" s="60" t="s">
         <v>220</v>
       </c>
-      <c r="E50" s="57" t="s">
+      <c r="E50" s="55" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="51" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B51" s="73"/>
+    <row r="51" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B51" s="74"/>
       <c r="C51" s="5" t="s">
         <v>583</v>
       </c>
       <c r="D51" s="31" t="s">
         <v>585</v>
       </c>
-      <c r="E51" s="83" t="s">
+      <c r="E51" s="81" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="52" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B52" s="73"/>
+    <row r="52" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B52" s="74"/>
       <c r="C52" s="5" t="s">
         <v>584</v>
       </c>
       <c r="D52" s="31" t="s">
         <v>586</v>
       </c>
-      <c r="E52" s="70"/>
-    </row>
-    <row r="53" spans="2:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B53" s="73"/>
+      <c r="E52" s="79"/>
+    </row>
+    <row r="53" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B53" s="74"/>
       <c r="C53" s="29" t="s">
         <v>634</v>
       </c>
-      <c r="D53" s="50" t="s">
+      <c r="D53" s="48" t="s">
         <v>419</v>
       </c>
-      <c r="E53" s="70"/>
-    </row>
-    <row r="54" spans="2:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B54" s="73"/>
+      <c r="E53" s="79"/>
+    </row>
+    <row r="54" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B54" s="74"/>
       <c r="C54" s="29" t="s">
         <v>351</v>
       </c>
-      <c r="D54" s="51" t="s">
+      <c r="D54" s="49" t="s">
         <v>418</v>
       </c>
-      <c r="E54" s="70"/>
-    </row>
-    <row r="55" spans="2:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B55" s="73"/>
+      <c r="E54" s="79"/>
+    </row>
+    <row r="55" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B55" s="74"/>
       <c r="C55" s="29" t="s">
         <v>350</v>
       </c>
-      <c r="D55" s="50" t="s">
+      <c r="D55" s="48" t="s">
         <v>420</v>
       </c>
-      <c r="E55" s="70"/>
-    </row>
-    <row r="56" spans="2:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B56" s="73"/>
+      <c r="E55" s="79"/>
+    </row>
+    <row r="56" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B56" s="74"/>
       <c r="C56" s="29" t="s">
         <v>633</v>
       </c>
-      <c r="D56" s="51" t="s">
+      <c r="D56" s="49" t="s">
         <v>354</v>
       </c>
-      <c r="E56" s="70"/>
-    </row>
-    <row r="57" spans="2:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B57" s="73"/>
+      <c r="E56" s="79"/>
+    </row>
+    <row r="57" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B57" s="74"/>
       <c r="C57" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="D57" s="51" t="s">
+      <c r="D57" s="49" t="s">
         <v>355</v>
       </c>
-      <c r="E57" s="70"/>
-    </row>
-    <row r="58" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B58" s="73"/>
+      <c r="E57" s="79"/>
+    </row>
+    <row r="58" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B58" s="74"/>
       <c r="C58" s="5" t="s">
         <v>312</v>
       </c>
       <c r="D58" s="29" t="s">
         <v>356</v>
       </c>
-      <c r="E58" s="70"/>
-    </row>
-    <row r="59" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B59" s="73"/>
+      <c r="E58" s="79"/>
+    </row>
+    <row r="59" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B59" s="74"/>
       <c r="C59" s="5" t="s">
         <v>311</v>
       </c>
       <c r="D59" s="29" t="s">
         <v>357</v>
       </c>
-      <c r="E59" s="70"/>
-    </row>
-    <row r="60" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B60" s="73"/>
+      <c r="E59" s="79"/>
+    </row>
+    <row r="60" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B60" s="74"/>
       <c r="C60" s="7" t="s">
         <v>310</v>
       </c>
       <c r="D60" s="29" t="s">
         <v>358</v>
       </c>
-      <c r="E60" s="70"/>
-    </row>
-    <row r="61" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B61" s="73"/>
+      <c r="E60" s="79"/>
+    </row>
+    <row r="61" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B61" s="74"/>
       <c r="C61" s="7" t="s">
         <v>309</v>
       </c>
       <c r="D61" s="29" t="s">
         <v>359</v>
       </c>
-      <c r="E61" s="70"/>
-    </row>
-    <row r="62" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B62" s="73"/>
+      <c r="E61" s="79"/>
+    </row>
+    <row r="62" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B62" s="74"/>
       <c r="C62" s="7" t="s">
         <v>308</v>
       </c>
       <c r="D62" s="29" t="s">
         <v>360</v>
       </c>
-      <c r="E62" s="70"/>
-    </row>
-    <row r="63" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B63" s="73"/>
+      <c r="E62" s="79"/>
+    </row>
+    <row r="63" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B63" s="74"/>
       <c r="C63" s="7" t="s">
         <v>307</v>
       </c>
       <c r="D63" s="29" t="s">
         <v>361</v>
       </c>
-      <c r="E63" s="70"/>
-    </row>
-    <row r="64" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B64" s="73"/>
+      <c r="E63" s="79"/>
+    </row>
+    <row r="64" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B64" s="74"/>
       <c r="C64" s="7" t="s">
         <v>306</v>
       </c>
       <c r="D64" s="29" t="s">
         <v>362</v>
       </c>
-      <c r="E64" s="70"/>
-    </row>
-    <row r="65" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B65" s="73"/>
+      <c r="E64" s="79"/>
+    </row>
+    <row r="65" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B65" s="74"/>
       <c r="C65" s="7" t="s">
         <v>305</v>
       </c>
       <c r="D65" s="29" t="s">
         <v>363</v>
       </c>
-      <c r="E65" s="70"/>
-    </row>
-    <row r="66" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B66" s="73"/>
+      <c r="E65" s="79"/>
+    </row>
+    <row r="66" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B66" s="74"/>
       <c r="C66" s="7" t="s">
         <v>304</v>
       </c>
       <c r="D66" s="29" t="s">
         <v>364</v>
       </c>
-      <c r="E66" s="70"/>
-    </row>
-    <row r="67" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B67" s="73"/>
+      <c r="E66" s="79"/>
+    </row>
+    <row r="67" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B67" s="74"/>
       <c r="C67" s="7" t="s">
         <v>303</v>
       </c>
       <c r="D67" s="29" t="s">
         <v>365</v>
       </c>
-      <c r="E67" s="70"/>
-    </row>
-    <row r="68" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B68" s="73"/>
+      <c r="E67" s="79"/>
+    </row>
+    <row r="68" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B68" s="74"/>
       <c r="C68" s="7" t="s">
         <v>302</v>
       </c>
       <c r="D68" s="29" t="s">
         <v>366</v>
       </c>
-      <c r="E68" s="70"/>
-    </row>
-    <row r="69" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B69" s="73"/>
+      <c r="E68" s="79"/>
+    </row>
+    <row r="69" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B69" s="74"/>
       <c r="C69" s="7" t="s">
         <v>301</v>
       </c>
       <c r="D69" s="29" t="s">
         <v>367</v>
       </c>
-      <c r="E69" s="70"/>
-    </row>
-    <row r="70" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B70" s="73"/>
+      <c r="E69" s="79"/>
+    </row>
+    <row r="70" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B70" s="74"/>
       <c r="C70" s="7" t="s">
         <v>299</v>
       </c>
       <c r="D70" s="29" t="s">
         <v>368</v>
       </c>
-      <c r="E70" s="70"/>
-    </row>
-    <row r="71" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B71" s="73"/>
+      <c r="E70" s="79"/>
+    </row>
+    <row r="71" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B71" s="74"/>
       <c r="C71" s="7" t="s">
         <v>298</v>
       </c>
       <c r="D71" s="29" t="s">
         <v>369</v>
       </c>
-      <c r="E71" s="70"/>
-    </row>
-    <row r="72" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B72" s="73"/>
+      <c r="E71" s="79"/>
+    </row>
+    <row r="72" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B72" s="74"/>
       <c r="C72" s="7" t="s">
         <v>300</v>
       </c>
       <c r="D72" s="29" t="s">
         <v>370</v>
       </c>
-      <c r="E72" s="70"/>
-    </row>
-    <row r="73" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B73" s="73"/>
+      <c r="E72" s="79"/>
+    </row>
+    <row r="73" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B73" s="74"/>
       <c r="C73" s="7" t="s">
         <v>313</v>
       </c>
       <c r="D73" s="29" t="s">
         <v>371</v>
       </c>
-      <c r="E73" s="70"/>
-    </row>
-    <row r="74" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B74" s="73"/>
+      <c r="E73" s="79"/>
+    </row>
+    <row r="74" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B74" s="74"/>
       <c r="C74" s="7" t="s">
         <v>314</v>
       </c>
       <c r="D74" s="29" t="s">
         <v>372</v>
       </c>
-      <c r="E74" s="70"/>
-    </row>
-    <row r="75" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B75" s="73"/>
+      <c r="E74" s="79"/>
+    </row>
+    <row r="75" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B75" s="74"/>
       <c r="C75" s="7" t="s">
         <v>315</v>
       </c>
       <c r="D75" s="31" t="s">
         <v>373</v>
       </c>
-      <c r="E75" s="86"/>
-    </row>
-    <row r="76" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B76" s="73"/>
+      <c r="E75" s="84"/>
+    </row>
+    <row r="76" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B76" s="74"/>
       <c r="C76" s="5" t="s">
         <v>111</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="E76" s="48"/>
-    </row>
-    <row r="77" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="74"/>
+      <c r="E76" s="11"/>
+    </row>
+    <row r="77" spans="2:5" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B77" s="77"/>
       <c r="C77" s="9" t="s">
         <v>112</v>
       </c>
       <c r="D77" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="E77" s="49"/>
-    </row>
-    <row r="78" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B78" s="73" t="s">
+      <c r="E77" s="17"/>
+    </row>
+    <row r="78" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B78" s="74" t="s">
         <v>132</v>
       </c>
       <c r="C78" s="25" t="s">
@@ -3742,8 +3741,8 @@
       </c>
       <c r="E78" s="12"/>
     </row>
-    <row r="79" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B79" s="73"/>
+    <row r="79" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B79" s="74"/>
       <c r="C79" s="39" t="s">
         <v>4</v>
       </c>
@@ -3752,8 +3751,8 @@
       </c>
       <c r="E79" s="12"/>
     </row>
-    <row r="80" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B80" s="73"/>
+    <row r="80" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B80" s="74"/>
       <c r="C80" s="14" t="s">
         <v>3</v>
       </c>
@@ -3762,20 +3761,20 @@
       </c>
       <c r="E80" s="12"/>
     </row>
-    <row r="81" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B81" s="73"/>
+    <row r="81" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B81" s="74"/>
       <c r="C81" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D81" s="47" t="s">
         <v>635</v>
       </c>
-      <c r="E81" s="87" t="s">
+      <c r="E81" s="67" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="82" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B82" s="73"/>
+    <row r="82" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B82" s="74"/>
       <c r="C82" s="14" t="s">
         <v>7</v>
       </c>
@@ -3784,8 +3783,8 @@
       </c>
       <c r="E82" s="12"/>
     </row>
-    <row r="83" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B83" s="73"/>
+    <row r="83" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B83" s="74"/>
       <c r="C83" s="14" t="s">
         <v>8</v>
       </c>
@@ -3794,20 +3793,20 @@
       </c>
       <c r="E83" s="12"/>
     </row>
-    <row r="84" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B84" s="73"/>
+    <row r="84" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B84" s="74"/>
       <c r="C84" s="38" t="s">
         <v>580</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>629</v>
       </c>
-      <c r="E84" s="88" t="s">
+      <c r="E84" s="68" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="85" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B85" s="73"/>
+    <row r="85" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B85" s="74"/>
       <c r="C85" s="14" t="s">
         <v>5</v>
       </c>
@@ -3816,8 +3815,8 @@
       </c>
       <c r="E85" s="12"/>
     </row>
-    <row r="86" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B86" s="73"/>
+    <row r="86" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B86" s="74"/>
       <c r="C86" s="38" t="s">
         <v>578</v>
       </c>
@@ -3826,8 +3825,8 @@
       </c>
       <c r="E86" s="12"/>
     </row>
-    <row r="87" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="73"/>
+    <row r="87" spans="2:5" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B87" s="74"/>
       <c r="C87" s="14" t="s">
         <v>6</v>
       </c>
@@ -3836,8 +3835,8 @@
       </c>
       <c r="E87" s="12"/>
     </row>
-    <row r="88" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="78" t="s">
+    <row r="88" spans="2:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B88" s="72" t="s">
         <v>424</v>
       </c>
       <c r="C88" s="35" t="s">
@@ -3846,31 +3845,31 @@
       <c r="D88" s="30" t="s">
         <v>426</v>
       </c>
-      <c r="E88" s="82" t="s">
+      <c r="E88" s="78" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="89" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="75"/>
+    <row r="89" spans="2:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B89" s="69"/>
       <c r="C89" s="14" t="s">
         <v>427</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="E89" s="70"/>
-    </row>
-    <row r="90" spans="2:5" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="79"/>
+      <c r="E89" s="79"/>
+    </row>
+    <row r="90" spans="2:5" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B90" s="73"/>
       <c r="C90" s="24" t="s">
         <v>428</v>
       </c>
       <c r="D90" s="9" t="s">
         <v>430</v>
       </c>
-      <c r="E90" s="71"/>
-    </row>
-    <row r="91" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="E90" s="80"/>
+    </row>
+    <row r="91" spans="2:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B91" s="42"/>
       <c r="C91" s="14" t="s">
         <v>43</v>
@@ -3878,9 +3877,9 @@
       <c r="D91" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E91" s="56"/>
-    </row>
-    <row r="92" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="E91" s="54"/>
+    </row>
+    <row r="92" spans="2:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B92" s="42"/>
       <c r="C92" s="14" t="s">
         <v>44</v>
@@ -3890,7 +3889,7 @@
       </c>
       <c r="E92" s="34"/>
     </row>
-    <row r="93" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B93" s="42"/>
       <c r="C93" s="14" t="s">
         <v>45</v>
@@ -3900,7 +3899,7 @@
       </c>
       <c r="E93" s="34"/>
     </row>
-    <row r="94" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B94" s="42"/>
       <c r="C94" s="14" t="s">
         <v>46</v>
@@ -3910,7 +3909,7 @@
       </c>
       <c r="E94" s="34"/>
     </row>
-    <row r="95" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B95" s="42"/>
       <c r="C95" s="14" t="s">
         <v>53</v>
@@ -3920,7 +3919,7 @@
       </c>
       <c r="E95" s="34"/>
     </row>
-    <row r="96" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B96" s="42"/>
       <c r="C96" s="14" t="s">
         <v>86</v>
@@ -3930,7 +3929,7 @@
       </c>
       <c r="E96" s="34"/>
     </row>
-    <row r="97" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B97" s="42"/>
       <c r="C97" s="14" t="s">
         <v>87</v>
@@ -3940,7 +3939,7 @@
       </c>
       <c r="E97" s="34"/>
     </row>
-    <row r="98" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B98" s="42"/>
       <c r="C98" s="14" t="s">
         <v>88</v>
@@ -3950,7 +3949,7 @@
       </c>
       <c r="E98" s="34"/>
     </row>
-    <row r="99" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B99" s="42"/>
       <c r="C99" s="14" t="s">
         <v>89</v>
@@ -3958,10 +3957,10 @@
       <c r="D99" s="29" t="s">
         <v>414</v>
       </c>
-      <c r="E99" s="57"/>
-    </row>
-    <row r="100" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B100" s="75" t="s">
+      <c r="E99" s="55"/>
+    </row>
+    <row r="100" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B100" s="69" t="s">
         <v>566</v>
       </c>
       <c r="C100" s="14" t="s">
@@ -3972,8 +3971,8 @@
       </c>
       <c r="E100" s="6"/>
     </row>
-    <row r="101" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B101" s="75"/>
+    <row r="101" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B101" s="69"/>
       <c r="C101" s="14" t="s">
         <v>85</v>
       </c>
@@ -3982,8 +3981,8 @@
       </c>
       <c r="E101" s="6"/>
     </row>
-    <row r="102" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B102" s="75"/>
+    <row r="102" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B102" s="69"/>
       <c r="C102" s="14" t="s">
         <v>33</v>
       </c>
@@ -3992,8 +3991,8 @@
       </c>
       <c r="E102" s="6"/>
     </row>
-    <row r="103" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B103" s="75"/>
+    <row r="103" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B103" s="69"/>
       <c r="C103" s="14" t="s">
         <v>34</v>
       </c>
@@ -4002,8 +4001,8 @@
       </c>
       <c r="E103" s="6"/>
     </row>
-    <row r="104" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B104" s="75"/>
+    <row r="104" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B104" s="69"/>
       <c r="C104" s="14" t="s">
         <v>35</v>
       </c>
@@ -4012,8 +4011,8 @@
       </c>
       <c r="E104" s="6"/>
     </row>
-    <row r="105" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B105" s="75"/>
+    <row r="105" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B105" s="69"/>
       <c r="C105" s="14" t="s">
         <v>36</v>
       </c>
@@ -4022,8 +4021,8 @@
       </c>
       <c r="E105" s="6"/>
     </row>
-    <row r="106" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B106" s="75"/>
+    <row r="106" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B106" s="69"/>
       <c r="C106" s="14" t="s">
         <v>54</v>
       </c>
@@ -4032,8 +4031,8 @@
       </c>
       <c r="E106" s="6"/>
     </row>
-    <row r="107" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B107" s="75"/>
+    <row r="107" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B107" s="69"/>
       <c r="C107" s="14" t="s">
         <v>48</v>
       </c>
@@ -4042,8 +4041,8 @@
       </c>
       <c r="E107" s="6"/>
     </row>
-    <row r="108" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B108" s="75"/>
+    <row r="108" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B108" s="69"/>
       <c r="C108" s="14" t="s">
         <v>90</v>
       </c>
@@ -4052,8 +4051,8 @@
       </c>
       <c r="E108" s="6"/>
     </row>
-    <row r="109" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B109" s="75"/>
+    <row r="109" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B109" s="69"/>
       <c r="C109" s="14" t="s">
         <v>69</v>
       </c>
@@ -4062,8 +4061,8 @@
       </c>
       <c r="E109" s="6"/>
     </row>
-    <row r="110" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B110" s="75"/>
+    <row r="110" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B110" s="69"/>
       <c r="C110" s="14" t="s">
         <v>70</v>
       </c>
@@ -4072,8 +4071,8 @@
       </c>
       <c r="E110" s="6"/>
     </row>
-    <row r="111" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B111" s="75"/>
+    <row r="111" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B111" s="69"/>
       <c r="C111" s="14" t="s">
         <v>71</v>
       </c>
@@ -4082,8 +4081,8 @@
       </c>
       <c r="E111" s="6"/>
     </row>
-    <row r="112" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B112" s="75"/>
+    <row r="112" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B112" s="69"/>
       <c r="C112" s="14" t="s">
         <v>72</v>
       </c>
@@ -4092,8 +4091,8 @@
       </c>
       <c r="E112" s="6"/>
     </row>
-    <row r="113" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B113" s="75"/>
+    <row r="113" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B113" s="69"/>
       <c r="C113" s="14" t="s">
         <v>73</v>
       </c>
@@ -4102,8 +4101,8 @@
       </c>
       <c r="E113" s="6"/>
     </row>
-    <row r="114" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B114" s="75"/>
+    <row r="114" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B114" s="69"/>
       <c r="C114" s="14" t="s">
         <v>83</v>
       </c>
@@ -4112,8 +4111,8 @@
       </c>
       <c r="E114" s="6"/>
     </row>
-    <row r="115" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B115" s="75"/>
+    <row r="115" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B115" s="69"/>
       <c r="C115" s="14" t="s">
         <v>77</v>
       </c>
@@ -4122,8 +4121,8 @@
       </c>
       <c r="E115" s="6"/>
     </row>
-    <row r="116" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B116" s="75"/>
+    <row r="116" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B116" s="69"/>
       <c r="C116" s="14" t="s">
         <v>76</v>
       </c>
@@ -4132,8 +4131,8 @@
       </c>
       <c r="E116" s="6"/>
     </row>
-    <row r="117" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B117" s="75"/>
+    <row r="117" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B117" s="69"/>
       <c r="C117" s="14" t="s">
         <v>75</v>
       </c>
@@ -4142,8 +4141,8 @@
       </c>
       <c r="E117" s="6"/>
     </row>
-    <row r="118" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B118" s="75"/>
+    <row r="118" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B118" s="69"/>
       <c r="C118" s="14" t="s">
         <v>67</v>
       </c>
@@ -4152,8 +4151,8 @@
       </c>
       <c r="E118" s="6"/>
     </row>
-    <row r="119" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B119" s="75"/>
+    <row r="119" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B119" s="69"/>
       <c r="C119" s="14" t="s">
         <v>66</v>
       </c>
@@ -4162,8 +4161,8 @@
       </c>
       <c r="E119" s="6"/>
     </row>
-    <row r="120" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B120" s="75"/>
+    <row r="120" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B120" s="69"/>
       <c r="C120" s="14" t="s">
         <v>68</v>
       </c>
@@ -4172,8 +4171,8 @@
       </c>
       <c r="E120" s="6"/>
     </row>
-    <row r="121" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B121" s="75"/>
+    <row r="121" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B121" s="69"/>
       <c r="C121" s="14" t="s">
         <v>41</v>
       </c>
@@ -4182,8 +4181,8 @@
       </c>
       <c r="E121" s="6"/>
     </row>
-    <row r="122" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B122" s="75"/>
+    <row r="122" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B122" s="69"/>
       <c r="C122" s="14" t="s">
         <v>30</v>
       </c>
@@ -4192,8 +4191,8 @@
       </c>
       <c r="E122" s="6"/>
     </row>
-    <row r="123" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B123" s="75"/>
+    <row r="123" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B123" s="69"/>
       <c r="C123" s="14" t="s">
         <v>31</v>
       </c>
@@ -4202,8 +4201,8 @@
       </c>
       <c r="E123" s="6"/>
     </row>
-    <row r="124" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B124" s="75"/>
+    <row r="124" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B124" s="69"/>
       <c r="C124" s="14" t="s">
         <v>32</v>
       </c>
@@ -4212,8 +4211,8 @@
       </c>
       <c r="E124" s="6"/>
     </row>
-    <row r="125" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B125" s="75"/>
+    <row r="125" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B125" s="69"/>
       <c r="C125" s="14" t="s">
         <v>47</v>
       </c>
@@ -4222,8 +4221,8 @@
       </c>
       <c r="E125" s="6"/>
     </row>
-    <row r="126" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B126" s="75"/>
+    <row r="126" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B126" s="69"/>
       <c r="C126" s="14" t="s">
         <v>42</v>
       </c>
@@ -4232,8 +4231,8 @@
       </c>
       <c r="E126" s="6"/>
     </row>
-    <row r="127" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B127" s="75"/>
+    <row r="127" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B127" s="69"/>
       <c r="C127" s="14" t="s">
         <v>74</v>
       </c>
@@ -4242,8 +4241,8 @@
       </c>
       <c r="E127" s="6"/>
     </row>
-    <row r="128" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B128" s="75"/>
+    <row r="128" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B128" s="69"/>
       <c r="C128" s="14" t="s">
         <v>65</v>
       </c>
@@ -4252,8 +4251,8 @@
       </c>
       <c r="E128" s="6"/>
     </row>
-    <row r="129" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B129" s="75"/>
+    <row r="129" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B129" s="69"/>
       <c r="C129" s="14" t="s">
         <v>52</v>
       </c>
@@ -4262,8 +4261,8 @@
       </c>
       <c r="E129" s="6"/>
     </row>
-    <row r="130" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B130" s="75"/>
+    <row r="130" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B130" s="69"/>
       <c r="C130" s="14" t="s">
         <v>78</v>
       </c>
@@ -4272,8 +4271,8 @@
       </c>
       <c r="E130" s="6"/>
     </row>
-    <row r="131" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B131" s="75"/>
+    <row r="131" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B131" s="69"/>
       <c r="C131" s="14" t="s">
         <v>79</v>
       </c>
@@ -4282,8 +4281,8 @@
       </c>
       <c r="E131" s="6"/>
     </row>
-    <row r="132" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B132" s="75"/>
+    <row r="132" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B132" s="69"/>
       <c r="C132" s="14" t="s">
         <v>80</v>
       </c>
@@ -4292,8 +4291,8 @@
       </c>
       <c r="E132" s="6"/>
     </row>
-    <row r="133" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B133" s="75"/>
+    <row r="133" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B133" s="69"/>
       <c r="C133" s="14" t="s">
         <v>81</v>
       </c>
@@ -4302,8 +4301,8 @@
       </c>
       <c r="E133" s="6"/>
     </row>
-    <row r="134" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B134" s="75"/>
+    <row r="134" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B134" s="69"/>
       <c r="C134" s="14" t="s">
         <v>82</v>
       </c>
@@ -4312,8 +4311,8 @@
       </c>
       <c r="E134" s="6"/>
     </row>
-    <row r="135" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B135" s="75"/>
+    <row r="135" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B135" s="69"/>
       <c r="C135" s="14" t="s">
         <v>84</v>
       </c>
@@ -4322,8 +4321,8 @@
       </c>
       <c r="E135" s="6"/>
     </row>
-    <row r="136" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B136" s="75"/>
+    <row r="136" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B136" s="69"/>
       <c r="C136" s="14" t="s">
         <v>29</v>
       </c>
@@ -4332,8 +4331,8 @@
       </c>
       <c r="E136" s="6"/>
     </row>
-    <row r="137" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B137" s="75"/>
+    <row r="137" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B137" s="69"/>
       <c r="C137" s="14" t="s">
         <v>55</v>
       </c>
@@ -4342,8 +4341,8 @@
       </c>
       <c r="E137" s="6"/>
     </row>
-    <row r="138" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B138" s="75"/>
+    <row r="138" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B138" s="69"/>
       <c r="C138" s="14" t="s">
         <v>56</v>
       </c>
@@ -4352,8 +4351,8 @@
       </c>
       <c r="E138" s="6"/>
     </row>
-    <row r="139" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B139" s="75"/>
+    <row r="139" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B139" s="69"/>
       <c r="C139" s="14" t="s">
         <v>57</v>
       </c>
@@ -4362,8 +4361,8 @@
       </c>
       <c r="E139" s="6"/>
     </row>
-    <row r="140" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B140" s="75"/>
+    <row r="140" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B140" s="69"/>
       <c r="C140" s="14" t="s">
         <v>58</v>
       </c>
@@ -4372,8 +4371,8 @@
       </c>
       <c r="E140" s="6"/>
     </row>
-    <row r="141" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B141" s="75"/>
+    <row r="141" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B141" s="69"/>
       <c r="C141" s="14" t="s">
         <v>59</v>
       </c>
@@ -4382,8 +4381,8 @@
       </c>
       <c r="E141" s="6"/>
     </row>
-    <row r="142" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B142" s="75"/>
+    <row r="142" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B142" s="69"/>
       <c r="C142" s="14" t="s">
         <v>60</v>
       </c>
@@ -4392,8 +4391,8 @@
       </c>
       <c r="E142" s="6"/>
     </row>
-    <row r="143" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B143" s="75"/>
+    <row r="143" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B143" s="69"/>
       <c r="C143" s="14" t="s">
         <v>61</v>
       </c>
@@ -4402,8 +4401,8 @@
       </c>
       <c r="E143" s="6"/>
     </row>
-    <row r="144" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B144" s="75"/>
+    <row r="144" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B144" s="69"/>
       <c r="C144" s="14" t="s">
         <v>62</v>
       </c>
@@ -4412,8 +4411,8 @@
       </c>
       <c r="E144" s="6"/>
     </row>
-    <row r="145" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B145" s="75"/>
+    <row r="145" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B145" s="69"/>
       <c r="C145" s="14" t="s">
         <v>63</v>
       </c>
@@ -4422,8 +4421,8 @@
       </c>
       <c r="E145" s="6"/>
     </row>
-    <row r="146" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B146" s="75"/>
+    <row r="146" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B146" s="69"/>
       <c r="C146" s="14" t="s">
         <v>64</v>
       </c>
@@ -4432,8 +4431,8 @@
       </c>
       <c r="E146" s="6"/>
     </row>
-    <row r="147" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B147" s="75"/>
+    <row r="147" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B147" s="69"/>
       <c r="C147" s="14" t="s">
         <v>49</v>
       </c>
@@ -4442,8 +4441,8 @@
       </c>
       <c r="E147" s="6"/>
     </row>
-    <row r="148" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B148" s="75"/>
+    <row r="148" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B148" s="69"/>
       <c r="C148" s="14" t="s">
         <v>50</v>
       </c>
@@ -4452,8 +4451,8 @@
       </c>
       <c r="E148" s="6"/>
     </row>
-    <row r="149" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B149" s="75"/>
+    <row r="149" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B149" s="69"/>
       <c r="C149" s="14" t="s">
         <v>51</v>
       </c>
@@ -4462,8 +4461,8 @@
       </c>
       <c r="E149" s="6"/>
     </row>
-    <row r="150" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B150" s="75"/>
+    <row r="150" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B150" s="69"/>
       <c r="C150" s="14" t="s">
         <v>37</v>
       </c>
@@ -4472,8 +4471,8 @@
       </c>
       <c r="E150" s="6"/>
     </row>
-    <row r="151" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B151" s="75"/>
+    <row r="151" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B151" s="69"/>
       <c r="C151" s="14" t="s">
         <v>38</v>
       </c>
@@ -4482,8 +4481,8 @@
       </c>
       <c r="E151" s="6"/>
     </row>
-    <row r="152" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B152" s="75"/>
+    <row r="152" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B152" s="69"/>
       <c r="C152" s="14" t="s">
         <v>39</v>
       </c>
@@ -4492,8 +4491,8 @@
       </c>
       <c r="E152" s="6"/>
     </row>
-    <row r="153" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B153" s="75"/>
+    <row r="153" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B153" s="69"/>
       <c r="C153" s="14" t="s">
         <v>40</v>
       </c>
@@ -4502,8 +4501,8 @@
       </c>
       <c r="E153" s="6"/>
     </row>
-    <row r="154" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="75"/>
+    <row r="154" spans="2:5" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B154" s="69"/>
       <c r="C154" s="15" t="s">
         <v>91</v>
       </c>
@@ -4512,342 +4511,342 @@
       </c>
       <c r="E154" s="6"/>
     </row>
-    <row r="155" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B155" s="72" t="s">
+    <row r="155" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B155" s="86" t="s">
         <v>340</v>
       </c>
       <c r="C155" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="D155" s="58" t="s">
+      <c r="D155" s="56" t="s">
         <v>381</v>
       </c>
-      <c r="E155" s="69" t="s">
+      <c r="E155" s="85" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="156" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B156" s="73"/>
+    <row r="156" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B156" s="74"/>
       <c r="C156" s="6" t="s">
         <v>343</v>
       </c>
       <c r="D156" s="27" t="s">
         <v>382</v>
       </c>
-      <c r="E156" s="70"/>
-    </row>
-    <row r="157" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B157" s="73"/>
+      <c r="E156" s="79"/>
+    </row>
+    <row r="157" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B157" s="74"/>
       <c r="C157" s="6" t="s">
         <v>341</v>
       </c>
       <c r="D157" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="E157" s="70"/>
-    </row>
-    <row r="158" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B158" s="73"/>
+      <c r="E157" s="79"/>
+    </row>
+    <row r="158" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B158" s="74"/>
       <c r="C158" s="6" t="s">
         <v>344</v>
       </c>
       <c r="D158" s="27" t="s">
         <v>383</v>
       </c>
-      <c r="E158" s="70"/>
-    </row>
-    <row r="159" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B159" s="73"/>
+      <c r="E158" s="79"/>
+    </row>
+    <row r="159" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B159" s="74"/>
       <c r="C159" s="6" t="s">
         <v>320</v>
       </c>
       <c r="D159" s="27" t="s">
         <v>390</v>
       </c>
-      <c r="E159" s="70"/>
-    </row>
-    <row r="160" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B160" s="73"/>
+      <c r="E159" s="79"/>
+    </row>
+    <row r="160" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B160" s="74"/>
       <c r="C160" s="6" t="s">
         <v>321</v>
       </c>
       <c r="D160" s="27" t="s">
         <v>391</v>
       </c>
-      <c r="E160" s="70"/>
-    </row>
-    <row r="161" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B161" s="73"/>
+      <c r="E160" s="79"/>
+    </row>
+    <row r="161" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B161" s="74"/>
       <c r="C161" s="6" t="s">
         <v>329</v>
       </c>
       <c r="D161" s="27" t="s">
         <v>399</v>
       </c>
-      <c r="E161" s="70"/>
-    </row>
-    <row r="162" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B162" s="73"/>
+      <c r="E161" s="79"/>
+    </row>
+    <row r="162" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B162" s="74"/>
       <c r="C162" s="6" t="s">
         <v>597</v>
       </c>
       <c r="D162" s="27" t="s">
         <v>598</v>
       </c>
-      <c r="E162" s="70"/>
-    </row>
-    <row r="163" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B163" s="73"/>
+      <c r="E162" s="79"/>
+    </row>
+    <row r="163" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B163" s="74"/>
       <c r="C163" s="6" t="s">
         <v>333</v>
       </c>
       <c r="D163" s="27" t="s">
         <v>403</v>
       </c>
-      <c r="E163" s="70"/>
-    </row>
-    <row r="164" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B164" s="73"/>
+      <c r="E163" s="79"/>
+    </row>
+    <row r="164" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B164" s="74"/>
       <c r="C164" s="6" t="s">
         <v>318</v>
       </c>
       <c r="D164" s="27" t="s">
         <v>388</v>
       </c>
-      <c r="E164" s="70"/>
-    </row>
-    <row r="165" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B165" s="73"/>
+      <c r="E164" s="79"/>
+    </row>
+    <row r="165" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B165" s="74"/>
       <c r="C165" s="6" t="s">
         <v>326</v>
       </c>
       <c r="D165" s="27" t="s">
         <v>396</v>
       </c>
-      <c r="E165" s="70"/>
-    </row>
-    <row r="166" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B166" s="73"/>
+      <c r="E165" s="79"/>
+    </row>
+    <row r="166" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B166" s="74"/>
       <c r="C166" s="6" t="s">
         <v>346</v>
       </c>
       <c r="D166" s="27" t="s">
         <v>385</v>
       </c>
-      <c r="E166" s="70"/>
-    </row>
-    <row r="167" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B167" s="73"/>
+      <c r="E166" s="79"/>
+    </row>
+    <row r="167" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B167" s="74"/>
       <c r="C167" s="6" t="s">
         <v>331</v>
       </c>
       <c r="D167" s="27" t="s">
         <v>401</v>
       </c>
-      <c r="E167" s="70"/>
-    </row>
-    <row r="168" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B168" s="73"/>
+      <c r="E167" s="79"/>
+    </row>
+    <row r="168" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B168" s="74"/>
       <c r="C168" s="6" t="s">
         <v>334</v>
       </c>
       <c r="D168" s="27" t="s">
         <v>404</v>
       </c>
-      <c r="E168" s="70"/>
-    </row>
-    <row r="169" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B169" s="73"/>
+      <c r="E168" s="79"/>
+    </row>
+    <row r="169" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B169" s="74"/>
       <c r="C169" s="6" t="s">
         <v>336</v>
       </c>
       <c r="D169" s="27" t="s">
         <v>406</v>
       </c>
-      <c r="E169" s="70"/>
-    </row>
-    <row r="170" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B170" s="73"/>
+      <c r="E169" s="79"/>
+    </row>
+    <row r="170" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B170" s="74"/>
       <c r="C170" s="6" t="s">
         <v>335</v>
       </c>
       <c r="D170" s="27" t="s">
         <v>405</v>
       </c>
-      <c r="E170" s="70"/>
-    </row>
-    <row r="171" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B171" s="73"/>
+      <c r="E170" s="79"/>
+    </row>
+    <row r="171" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B171" s="74"/>
       <c r="C171" s="6" t="s">
         <v>323</v>
       </c>
       <c r="D171" s="27" t="s">
         <v>393</v>
       </c>
-      <c r="E171" s="70"/>
-    </row>
-    <row r="172" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B172" s="73"/>
+      <c r="E171" s="79"/>
+    </row>
+    <row r="172" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B172" s="74"/>
       <c r="C172" s="6" t="s">
         <v>325</v>
       </c>
       <c r="D172" s="27" t="s">
         <v>395</v>
       </c>
-      <c r="E172" s="70"/>
-    </row>
-    <row r="173" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B173" s="73"/>
+      <c r="E172" s="79"/>
+    </row>
+    <row r="173" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B173" s="74"/>
       <c r="C173" s="6" t="s">
         <v>328</v>
       </c>
       <c r="D173" s="27" t="s">
         <v>398</v>
       </c>
-      <c r="E173" s="70"/>
-    </row>
-    <row r="174" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B174" s="73"/>
+      <c r="E173" s="79"/>
+    </row>
+    <row r="174" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B174" s="74"/>
       <c r="C174" s="6" t="s">
         <v>327</v>
       </c>
       <c r="D174" s="27" t="s">
         <v>397</v>
       </c>
-      <c r="E174" s="70"/>
-    </row>
-    <row r="175" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B175" s="73"/>
+      <c r="E174" s="79"/>
+    </row>
+    <row r="175" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B175" s="74"/>
       <c r="C175" s="6" t="s">
         <v>595</v>
       </c>
       <c r="D175" s="27" t="s">
         <v>596</v>
       </c>
-      <c r="E175" s="70"/>
-    </row>
-    <row r="176" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B176" s="73"/>
+      <c r="E175" s="79"/>
+    </row>
+    <row r="176" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B176" s="74"/>
       <c r="C176" s="6" t="s">
         <v>593</v>
       </c>
       <c r="D176" s="27" t="s">
         <v>594</v>
       </c>
-      <c r="E176" s="70"/>
-    </row>
-    <row r="177" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B177" s="73"/>
+      <c r="E176" s="79"/>
+    </row>
+    <row r="177" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B177" s="74"/>
       <c r="C177" s="6" t="s">
         <v>332</v>
       </c>
       <c r="D177" s="27" t="s">
         <v>402</v>
       </c>
-      <c r="E177" s="70"/>
-    </row>
-    <row r="178" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B178" s="73"/>
+      <c r="E177" s="79"/>
+    </row>
+    <row r="178" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B178" s="74"/>
       <c r="C178" s="6" t="s">
         <v>322</v>
       </c>
       <c r="D178" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="E178" s="70"/>
-    </row>
-    <row r="179" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B179" s="73"/>
+      <c r="E178" s="79"/>
+    </row>
+    <row r="179" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B179" s="74"/>
       <c r="C179" s="6" t="s">
         <v>339</v>
       </c>
       <c r="D179" s="27" t="s">
         <v>409</v>
       </c>
-      <c r="E179" s="70"/>
-    </row>
-    <row r="180" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B180" s="73"/>
+      <c r="E179" s="79"/>
+    </row>
+    <row r="180" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B180" s="74"/>
       <c r="C180" s="6" t="s">
         <v>319</v>
       </c>
       <c r="D180" s="27" t="s">
         <v>389</v>
       </c>
-      <c r="E180" s="70"/>
-    </row>
-    <row r="181" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B181" s="73"/>
+      <c r="E180" s="79"/>
+    </row>
+    <row r="181" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B181" s="74"/>
       <c r="C181" s="6" t="s">
         <v>432</v>
       </c>
       <c r="D181" s="27" t="s">
         <v>386</v>
       </c>
-      <c r="E181" s="70"/>
-    </row>
-    <row r="182" spans="2:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B182" s="73"/>
+      <c r="E181" s="79"/>
+    </row>
+    <row r="182" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B182" s="74"/>
       <c r="C182" s="34" t="s">
         <v>317</v>
       </c>
       <c r="D182" s="27" t="s">
         <v>387</v>
       </c>
-      <c r="E182" s="70"/>
-    </row>
-    <row r="183" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B183" s="73"/>
+      <c r="E182" s="79"/>
+    </row>
+    <row r="183" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B183" s="74"/>
       <c r="C183" s="6" t="s">
         <v>324</v>
       </c>
       <c r="D183" s="27" t="s">
         <v>394</v>
       </c>
-      <c r="E183" s="70"/>
-    </row>
-    <row r="184" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B184" s="73"/>
+      <c r="E183" s="79"/>
+    </row>
+    <row r="184" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B184" s="74"/>
       <c r="C184" s="6" t="s">
         <v>345</v>
       </c>
       <c r="D184" s="27" t="s">
         <v>384</v>
       </c>
-      <c r="E184" s="70"/>
-    </row>
-    <row r="185" spans="2:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B185" s="73"/>
+      <c r="E184" s="79"/>
+    </row>
+    <row r="185" spans="2:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B185" s="74"/>
       <c r="C185" s="6" t="s">
         <v>337</v>
       </c>
       <c r="D185" s="27" t="s">
         <v>407</v>
       </c>
-      <c r="E185" s="70"/>
-    </row>
-    <row r="186" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B186" s="73"/>
+      <c r="E185" s="79"/>
+    </row>
+    <row r="186" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B186" s="74"/>
       <c r="C186" s="6" t="s">
         <v>338</v>
       </c>
       <c r="D186" s="27" t="s">
         <v>408</v>
       </c>
-      <c r="E186" s="70"/>
-    </row>
-    <row r="187" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B187" s="74"/>
+      <c r="E186" s="79"/>
+    </row>
+    <row r="187" spans="2:5" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B187" s="77"/>
       <c r="C187" s="13" t="s">
         <v>330</v>
       </c>
       <c r="D187" s="28" t="s">
         <v>400</v>
       </c>
-      <c r="E187" s="71"/>
-    </row>
-    <row r="188" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B188" s="73" t="s">
+      <c r="E187" s="80"/>
+    </row>
+    <row r="188" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B188" s="74" t="s">
         <v>636</v>
       </c>
       <c r="C188" s="3" t="s">
@@ -4858,8 +4857,8 @@
       </c>
       <c r="E188" s="6"/>
     </row>
-    <row r="189" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B189" s="73"/>
+    <row r="189" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B189" s="74"/>
       <c r="C189" s="5" t="s">
         <v>24</v>
       </c>
@@ -4868,8 +4867,8 @@
       </c>
       <c r="E189" s="6"/>
     </row>
-    <row r="190" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B190" s="73"/>
+    <row r="190" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B190" s="74"/>
       <c r="C190" s="5" t="s">
         <v>25</v>
       </c>
@@ -4878,8 +4877,8 @@
       </c>
       <c r="E190" s="8"/>
     </row>
-    <row r="191" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B191" s="74"/>
+    <row r="191" spans="2:5" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B191" s="77"/>
       <c r="C191" s="9" t="s">
         <v>0</v>
       </c>
@@ -4888,8 +4887,8 @@
       </c>
       <c r="E191" s="13"/>
     </row>
-    <row r="192" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B192" s="73" t="s">
+    <row r="192" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B192" s="74" t="s">
         <v>567</v>
       </c>
       <c r="C192" s="30" t="s">
@@ -4900,20 +4899,20 @@
       </c>
       <c r="E192" s="6"/>
     </row>
-    <row r="193" spans="2:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B193" s="73"/>
-      <c r="C193" s="62" t="s">
+    <row r="193" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B193" s="74"/>
+      <c r="C193" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="D193" s="52" t="s">
+      <c r="D193" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="E193" s="57" t="s">
+      <c r="E193" s="55" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="194" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B194" s="73"/>
+    <row r="194" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B194" s="74"/>
       <c r="C194" s="5" t="s">
         <v>591</v>
       </c>
@@ -4922,8 +4921,8 @@
       </c>
       <c r="E194" s="6"/>
     </row>
-    <row r="195" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B195" s="73"/>
+    <row r="195" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B195" s="74"/>
       <c r="C195" s="5" t="s">
         <v>433</v>
       </c>
@@ -4932,8 +4931,8 @@
       </c>
       <c r="E195" s="6"/>
     </row>
-    <row r="196" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B196" s="73"/>
+    <row r="196" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B196" s="74"/>
       <c r="C196" s="9" t="s">
         <v>26</v>
       </c>
@@ -4942,11 +4941,11 @@
       </c>
       <c r="E196" s="6"/>
     </row>
-    <row r="197" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B197" s="72" t="s">
+    <row r="197" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B197" s="86" t="s">
         <v>122</v>
       </c>
-      <c r="C197" s="59" t="s">
+      <c r="C197" s="57" t="s">
         <v>435</v>
       </c>
       <c r="D197" s="19" t="s">
@@ -4954,8 +4953,8 @@
       </c>
       <c r="E197" s="19"/>
     </row>
-    <row r="198" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B198" s="73"/>
+    <row r="198" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B198" s="74"/>
       <c r="C198" s="16" t="s">
         <v>436</v>
       </c>
@@ -4964,8 +4963,8 @@
       </c>
       <c r="E198" s="11"/>
     </row>
-    <row r="199" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B199" s="73"/>
+    <row r="199" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B199" s="74"/>
       <c r="C199" s="16" t="s">
         <v>437</v>
       </c>
@@ -4974,8 +4973,8 @@
       </c>
       <c r="E199" s="11"/>
     </row>
-    <row r="200" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B200" s="73"/>
+    <row r="200" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B200" s="74"/>
       <c r="C200" s="16" t="s">
         <v>438</v>
       </c>
@@ -4984,8 +4983,8 @@
       </c>
       <c r="E200" s="11"/>
     </row>
-    <row r="201" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B201" s="73"/>
+    <row r="201" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B201" s="74"/>
       <c r="C201" s="16" t="s">
         <v>440</v>
       </c>
@@ -4994,8 +4993,8 @@
       </c>
       <c r="E201" s="11"/>
     </row>
-    <row r="202" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B202" s="73"/>
+    <row r="202" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B202" s="74"/>
       <c r="C202" s="16" t="s">
         <v>599</v>
       </c>
@@ -5004,8 +5003,8 @@
       </c>
       <c r="E202" s="11"/>
     </row>
-    <row r="203" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B203" s="73"/>
+    <row r="203" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B203" s="74"/>
       <c r="C203" s="16" t="s">
         <v>441</v>
       </c>
@@ -5014,8 +5013,8 @@
       </c>
       <c r="E203" s="11"/>
     </row>
-    <row r="204" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B204" s="73"/>
+    <row r="204" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B204" s="74"/>
       <c r="C204" s="16" t="s">
         <v>443</v>
       </c>
@@ -5024,8 +5023,8 @@
       </c>
       <c r="E204" s="11"/>
     </row>
-    <row r="205" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B205" s="73"/>
+    <row r="205" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B205" s="74"/>
       <c r="C205" s="16" t="s">
         <v>444</v>
       </c>
@@ -5034,8 +5033,8 @@
       </c>
       <c r="E205" s="11"/>
     </row>
-    <row r="206" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B206" s="73"/>
+    <row r="206" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B206" s="74"/>
       <c r="C206" s="16" t="s">
         <v>446</v>
       </c>
@@ -5044,8 +5043,8 @@
       </c>
       <c r="E206" s="11"/>
     </row>
-    <row r="207" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B207" s="73"/>
+    <row r="207" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B207" s="74"/>
       <c r="C207" s="16" t="s">
         <v>448</v>
       </c>
@@ -5054,8 +5053,8 @@
       </c>
       <c r="E207" s="11"/>
     </row>
-    <row r="208" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B208" s="73"/>
+    <row r="208" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B208" s="74"/>
       <c r="C208" s="16" t="s">
         <v>449</v>
       </c>
@@ -5064,8 +5063,8 @@
       </c>
       <c r="E208" s="11"/>
     </row>
-    <row r="209" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B209" s="73"/>
+    <row r="209" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B209" s="74"/>
       <c r="C209" s="16" t="s">
         <v>450</v>
       </c>
@@ -5074,8 +5073,8 @@
       </c>
       <c r="E209" s="11"/>
     </row>
-    <row r="210" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B210" s="73"/>
+    <row r="210" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B210" s="74"/>
       <c r="C210" s="16" t="s">
         <v>601</v>
       </c>
@@ -5084,8 +5083,8 @@
       </c>
       <c r="E210" s="11"/>
     </row>
-    <row r="211" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B211" s="73"/>
+    <row r="211" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B211" s="74"/>
       <c r="C211" s="16" t="s">
         <v>451</v>
       </c>
@@ -5094,8 +5093,8 @@
       </c>
       <c r="E211" s="11"/>
     </row>
-    <row r="212" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B212" s="73"/>
+    <row r="212" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B212" s="74"/>
       <c r="C212" s="16" t="s">
         <v>452</v>
       </c>
@@ -5104,8 +5103,8 @@
       </c>
       <c r="E212" s="11"/>
     </row>
-    <row r="213" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B213" s="73"/>
+    <row r="213" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B213" s="74"/>
       <c r="C213" s="16" t="s">
         <v>453</v>
       </c>
@@ -5114,8 +5113,8 @@
       </c>
       <c r="E213" s="11"/>
     </row>
-    <row r="214" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B214" s="73"/>
+    <row r="214" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B214" s="74"/>
       <c r="C214" s="16" t="s">
         <v>456</v>
       </c>
@@ -5124,8 +5123,8 @@
       </c>
       <c r="E214" s="11"/>
     </row>
-    <row r="215" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B215" s="73"/>
+    <row r="215" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B215" s="74"/>
       <c r="C215" s="16" t="s">
         <v>457</v>
       </c>
@@ -5134,8 +5133,8 @@
       </c>
       <c r="E215" s="11"/>
     </row>
-    <row r="216" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B216" s="73"/>
+    <row r="216" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B216" s="74"/>
       <c r="C216" s="16" t="s">
         <v>459</v>
       </c>
@@ -5144,8 +5143,8 @@
       </c>
       <c r="E216" s="11"/>
     </row>
-    <row r="217" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B217" s="73"/>
+    <row r="217" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B217" s="74"/>
       <c r="C217" s="16" t="s">
         <v>460</v>
       </c>
@@ -5154,8 +5153,8 @@
       </c>
       <c r="E217" s="11"/>
     </row>
-    <row r="218" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B218" s="73"/>
+    <row r="218" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B218" s="74"/>
       <c r="C218" s="16" t="s">
         <v>462</v>
       </c>
@@ -5164,8 +5163,8 @@
       </c>
       <c r="E218" s="11"/>
     </row>
-    <row r="219" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B219" s="73"/>
+    <row r="219" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B219" s="74"/>
       <c r="C219" s="16" t="s">
         <v>464</v>
       </c>
@@ -5174,8 +5173,8 @@
       </c>
       <c r="E219" s="11"/>
     </row>
-    <row r="220" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B220" s="73"/>
+    <row r="220" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B220" s="74"/>
       <c r="C220" s="16" t="s">
         <v>466</v>
       </c>
@@ -5184,8 +5183,8 @@
       </c>
       <c r="E220" s="11"/>
     </row>
-    <row r="221" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B221" s="73"/>
+    <row r="221" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B221" s="74"/>
       <c r="C221" s="16" t="s">
         <v>468</v>
       </c>
@@ -5194,8 +5193,8 @@
       </c>
       <c r="E221" s="11"/>
     </row>
-    <row r="222" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B222" s="73"/>
+    <row r="222" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B222" s="74"/>
       <c r="C222" s="33" t="s">
         <v>623</v>
       </c>
@@ -5204,8 +5203,8 @@
       </c>
       <c r="E222" s="11"/>
     </row>
-    <row r="223" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B223" s="73"/>
+    <row r="223" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B223" s="74"/>
       <c r="C223" s="33" t="s">
         <v>625</v>
       </c>
@@ -5214,8 +5213,8 @@
       </c>
       <c r="E223" s="11"/>
     </row>
-    <row r="224" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B224" s="73"/>
+    <row r="224" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B224" s="74"/>
       <c r="C224" s="33" t="s">
         <v>609</v>
       </c>
@@ -5224,8 +5223,8 @@
       </c>
       <c r="E224" s="11"/>
     </row>
-    <row r="225" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B225" s="73"/>
+    <row r="225" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B225" s="74"/>
       <c r="C225" s="33" t="s">
         <v>611</v>
       </c>
@@ -5234,8 +5233,8 @@
       </c>
       <c r="E225" s="11"/>
     </row>
-    <row r="226" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B226" s="73"/>
+    <row r="226" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B226" s="74"/>
       <c r="C226" s="36" t="s">
         <v>475</v>
       </c>
@@ -5244,8 +5243,8 @@
       </c>
       <c r="E226" s="11"/>
     </row>
-    <row r="227" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B227" s="73"/>
+    <row r="227" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B227" s="74"/>
       <c r="C227" s="36" t="s">
         <v>477</v>
       </c>
@@ -5254,8 +5253,8 @@
       </c>
       <c r="E227" s="11"/>
     </row>
-    <row r="228" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B228" s="73"/>
+    <row r="228" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B228" s="74"/>
       <c r="C228" s="36" t="s">
         <v>479</v>
       </c>
@@ -5264,8 +5263,8 @@
       </c>
       <c r="E228" s="11"/>
     </row>
-    <row r="229" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B229" s="73"/>
+    <row r="229" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B229" s="74"/>
       <c r="C229" s="36" t="s">
         <v>481</v>
       </c>
@@ -5274,8 +5273,8 @@
       </c>
       <c r="E229" s="11"/>
     </row>
-    <row r="230" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B230" s="73"/>
+    <row r="230" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B230" s="74"/>
       <c r="C230" s="36" t="s">
         <v>483</v>
       </c>
@@ -5284,8 +5283,8 @@
       </c>
       <c r="E230" s="11"/>
     </row>
-    <row r="231" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B231" s="73"/>
+    <row r="231" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B231" s="74"/>
       <c r="C231" s="36" t="s">
         <v>485</v>
       </c>
@@ -5294,8 +5293,8 @@
       </c>
       <c r="E231" s="11"/>
     </row>
-    <row r="232" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B232" s="73"/>
+    <row r="232" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B232" s="74"/>
       <c r="C232" s="36" t="s">
         <v>487</v>
       </c>
@@ -5304,8 +5303,8 @@
       </c>
       <c r="E232" s="11"/>
     </row>
-    <row r="233" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B233" s="73"/>
+    <row r="233" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B233" s="74"/>
       <c r="C233" s="36" t="s">
         <v>490</v>
       </c>
@@ -5314,8 +5313,8 @@
       </c>
       <c r="E233" s="11"/>
     </row>
-    <row r="234" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B234" s="73"/>
+    <row r="234" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B234" s="74"/>
       <c r="C234" s="36" t="s">
         <v>491</v>
       </c>
@@ -5324,8 +5323,8 @@
       </c>
       <c r="E234" s="11"/>
     </row>
-    <row r="235" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B235" s="73"/>
+    <row r="235" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B235" s="74"/>
       <c r="C235" s="11" t="s">
         <v>493</v>
       </c>
@@ -5334,8 +5333,8 @@
       </c>
       <c r="E235" s="11"/>
     </row>
-    <row r="236" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B236" s="73"/>
+    <row r="236" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B236" s="74"/>
       <c r="C236" s="36" t="s">
         <v>495</v>
       </c>
@@ -5344,8 +5343,8 @@
       </c>
       <c r="E236" s="11"/>
     </row>
-    <row r="237" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B237" s="73"/>
+    <row r="237" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B237" s="74"/>
       <c r="C237" s="16" t="s">
         <v>470</v>
       </c>
@@ -5354,8 +5353,8 @@
       </c>
       <c r="E237" s="11"/>
     </row>
-    <row r="238" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B238" s="73"/>
+    <row r="238" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B238" s="74"/>
       <c r="C238" s="16" t="s">
         <v>469</v>
       </c>
@@ -5364,8 +5363,8 @@
       </c>
       <c r="E238" s="11"/>
     </row>
-    <row r="239" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B239" s="73"/>
+    <row r="239" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B239" s="74"/>
       <c r="C239" s="16" t="s">
         <v>471</v>
       </c>
@@ -5374,8 +5373,8 @@
       </c>
       <c r="E239" s="11"/>
     </row>
-    <row r="240" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B240" s="73"/>
+    <row r="240" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B240" s="74"/>
       <c r="C240" s="16" t="s">
         <v>472</v>
       </c>
@@ -5384,8 +5383,8 @@
       </c>
       <c r="E240" s="11"/>
     </row>
-    <row r="241" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B241" s="73"/>
+    <row r="241" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B241" s="74"/>
       <c r="C241" s="16" t="s">
         <v>473</v>
       </c>
@@ -5394,8 +5393,8 @@
       </c>
       <c r="E241" s="11"/>
     </row>
-    <row r="242" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B242" s="73"/>
+    <row r="242" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B242" s="74"/>
       <c r="C242" s="16" t="s">
         <v>474</v>
       </c>
@@ -5404,8 +5403,8 @@
       </c>
       <c r="E242" s="11"/>
     </row>
-    <row r="243" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B243" s="73"/>
+    <row r="243" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B243" s="74"/>
       <c r="C243" s="36" t="s">
         <v>497</v>
       </c>
@@ -5414,8 +5413,8 @@
       </c>
       <c r="E243" s="11"/>
     </row>
-    <row r="244" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B244" s="73"/>
+    <row r="244" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B244" s="74"/>
       <c r="C244" s="36" t="s">
         <v>499</v>
       </c>
@@ -5424,8 +5423,8 @@
       </c>
       <c r="E244" s="11"/>
     </row>
-    <row r="245" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B245" s="73"/>
+    <row r="245" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B245" s="74"/>
       <c r="C245" s="11" t="s">
         <v>501</v>
       </c>
@@ -5434,8 +5433,8 @@
       </c>
       <c r="E245" s="11"/>
     </row>
-    <row r="246" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B246" s="73"/>
+    <row r="246" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B246" s="74"/>
       <c r="C246" s="33" t="s">
         <v>503</v>
       </c>
@@ -5444,8 +5443,8 @@
       </c>
       <c r="E246" s="11"/>
     </row>
-    <row r="247" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B247" s="73"/>
+    <row r="247" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B247" s="74"/>
       <c r="C247" s="33" t="s">
         <v>509</v>
       </c>
@@ -5454,8 +5453,8 @@
       </c>
       <c r="E247" s="11"/>
     </row>
-    <row r="248" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B248" s="73"/>
+    <row r="248" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B248" s="74"/>
       <c r="C248" s="33" t="s">
         <v>508</v>
       </c>
@@ -5464,8 +5463,8 @@
       </c>
       <c r="E248" s="11"/>
     </row>
-    <row r="249" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B249" s="73"/>
+    <row r="249" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B249" s="74"/>
       <c r="C249" s="16" t="s">
         <v>504</v>
       </c>
@@ -5474,8 +5473,8 @@
       </c>
       <c r="E249" s="11"/>
     </row>
-    <row r="250" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B250" s="73"/>
+    <row r="250" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B250" s="74"/>
       <c r="C250" s="16" t="s">
         <v>506</v>
       </c>
@@ -5484,8 +5483,8 @@
       </c>
       <c r="E250" s="11"/>
     </row>
-    <row r="251" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B251" s="73"/>
+    <row r="251" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B251" s="74"/>
       <c r="C251" s="33" t="s">
         <v>510</v>
       </c>
@@ -5494,8 +5493,8 @@
       </c>
       <c r="E251" s="11"/>
     </row>
-    <row r="252" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B252" s="73"/>
+    <row r="252" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B252" s="74"/>
       <c r="C252" s="33" t="s">
         <v>511</v>
       </c>
@@ -5504,8 +5503,8 @@
       </c>
       <c r="E252" s="11"/>
     </row>
-    <row r="253" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B253" s="73"/>
+    <row r="253" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B253" s="74"/>
       <c r="C253" s="33" t="s">
         <v>512</v>
       </c>
@@ -5514,8 +5513,8 @@
       </c>
       <c r="E253" s="11"/>
     </row>
-    <row r="254" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B254" s="73"/>
+    <row r="254" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B254" s="74"/>
       <c r="C254" s="33" t="s">
         <v>513</v>
       </c>
@@ -5524,8 +5523,8 @@
       </c>
       <c r="E254" s="11"/>
     </row>
-    <row r="255" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B255" s="73"/>
+    <row r="255" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B255" s="74"/>
       <c r="C255" s="33" t="s">
         <v>514</v>
       </c>
@@ -5534,8 +5533,8 @@
       </c>
       <c r="E255" s="11"/>
     </row>
-    <row r="256" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B256" s="73"/>
+    <row r="256" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B256" s="74"/>
       <c r="C256" s="33" t="s">
         <v>515</v>
       </c>
@@ -5544,8 +5543,8 @@
       </c>
       <c r="E256" s="11"/>
     </row>
-    <row r="257" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B257" s="73"/>
+    <row r="257" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B257" s="74"/>
       <c r="C257" s="33" t="s">
         <v>516</v>
       </c>
@@ -5554,8 +5553,8 @@
       </c>
       <c r="E257" s="11"/>
     </row>
-    <row r="258" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B258" s="73"/>
+    <row r="258" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B258" s="74"/>
       <c r="C258" s="33" t="s">
         <v>517</v>
       </c>
@@ -5564,8 +5563,8 @@
       </c>
       <c r="E258" s="11"/>
     </row>
-    <row r="259" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B259" s="73"/>
+    <row r="259" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B259" s="74"/>
       <c r="C259" s="33" t="s">
         <v>518</v>
       </c>
@@ -5574,8 +5573,8 @@
       </c>
       <c r="E259" s="11"/>
     </row>
-    <row r="260" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B260" s="73"/>
+    <row r="260" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B260" s="74"/>
       <c r="C260" s="33" t="s">
         <v>520</v>
       </c>
@@ -5584,8 +5583,8 @@
       </c>
       <c r="E260" s="11"/>
     </row>
-    <row r="261" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B261" s="73"/>
+    <row r="261" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B261" s="74"/>
       <c r="C261" s="33" t="s">
         <v>522</v>
       </c>
@@ -5594,8 +5593,8 @@
       </c>
       <c r="E261" s="11"/>
     </row>
-    <row r="262" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B262" s="73"/>
+    <row r="262" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B262" s="74"/>
       <c r="C262" s="33" t="s">
         <v>524</v>
       </c>
@@ -5604,8 +5603,8 @@
       </c>
       <c r="E262" s="11"/>
     </row>
-    <row r="263" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B263" s="73"/>
+    <row r="263" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B263" s="74"/>
       <c r="C263" s="33" t="s">
         <v>526</v>
       </c>
@@ -5614,8 +5613,8 @@
       </c>
       <c r="E263" s="11"/>
     </row>
-    <row r="264" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B264" s="73"/>
+    <row r="264" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B264" s="74"/>
       <c r="C264" s="33" t="s">
         <v>527</v>
       </c>
@@ -5624,8 +5623,8 @@
       </c>
       <c r="E264" s="11"/>
     </row>
-    <row r="265" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B265" s="73"/>
+    <row r="265" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B265" s="74"/>
       <c r="C265" s="33" t="s">
         <v>533</v>
       </c>
@@ -5634,8 +5633,8 @@
       </c>
       <c r="E265" s="11"/>
     </row>
-    <row r="266" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B266" s="73"/>
+    <row r="266" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B266" s="74"/>
       <c r="C266" s="16" t="s">
         <v>529</v>
       </c>
@@ -5644,8 +5643,8 @@
       </c>
       <c r="E266" s="11"/>
     </row>
-    <row r="267" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B267" s="73"/>
+    <row r="267" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B267" s="74"/>
       <c r="C267" s="16" t="s">
         <v>531</v>
       </c>
@@ -5654,8 +5653,8 @@
       </c>
       <c r="E267" s="11"/>
     </row>
-    <row r="268" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B268" s="73"/>
+    <row r="268" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B268" s="74"/>
       <c r="C268" s="16" t="s">
         <v>534</v>
       </c>
@@ -5664,8 +5663,8 @@
       </c>
       <c r="E268" s="11"/>
     </row>
-    <row r="269" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B269" s="73"/>
+    <row r="269" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B269" s="74"/>
       <c r="C269" s="16" t="s">
         <v>536</v>
       </c>
@@ -5674,8 +5673,8 @@
       </c>
       <c r="E269" s="11"/>
     </row>
-    <row r="270" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B270" s="73"/>
+    <row r="270" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B270" s="74"/>
       <c r="C270" s="33" t="s">
         <v>538</v>
       </c>
@@ -5684,8 +5683,8 @@
       </c>
       <c r="E270" s="11"/>
     </row>
-    <row r="271" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B271" s="73"/>
+    <row r="271" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B271" s="74"/>
       <c r="C271" s="33" t="s">
         <v>613</v>
       </c>
@@ -5694,8 +5693,8 @@
       </c>
       <c r="E271" s="11"/>
     </row>
-    <row r="272" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B272" s="73"/>
+    <row r="272" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B272" s="74"/>
       <c r="C272" s="33" t="s">
         <v>603</v>
       </c>
@@ -5704,8 +5703,8 @@
       </c>
       <c r="E272" s="11"/>
     </row>
-    <row r="273" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B273" s="73"/>
+    <row r="273" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B273" s="74"/>
       <c r="C273" s="33" t="s">
         <v>539</v>
       </c>
@@ -5714,8 +5713,8 @@
       </c>
       <c r="E273" s="11"/>
     </row>
-    <row r="274" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B274" s="73"/>
+    <row r="274" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B274" s="74"/>
       <c r="C274" s="33" t="s">
         <v>617</v>
       </c>
@@ -5724,8 +5723,8 @@
       </c>
       <c r="E274" s="11"/>
     </row>
-    <row r="275" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B275" s="73"/>
+    <row r="275" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B275" s="74"/>
       <c r="C275" s="33" t="s">
         <v>621</v>
       </c>
@@ -5734,8 +5733,8 @@
       </c>
       <c r="E275" s="11"/>
     </row>
-    <row r="276" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B276" s="73"/>
+    <row r="276" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B276" s="74"/>
       <c r="C276" s="33" t="s">
         <v>619</v>
       </c>
@@ -5744,8 +5743,8 @@
       </c>
       <c r="E276" s="11"/>
     </row>
-    <row r="277" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B277" s="73"/>
+    <row r="277" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B277" s="74"/>
       <c r="C277" s="33" t="s">
         <v>615</v>
       </c>
@@ -5754,8 +5753,8 @@
       </c>
       <c r="E277" s="11"/>
     </row>
-    <row r="278" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B278" s="73"/>
+    <row r="278" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B278" s="74"/>
       <c r="C278" s="33" t="s">
         <v>540</v>
       </c>
@@ -5764,8 +5763,8 @@
       </c>
       <c r="E278" s="11"/>
     </row>
-    <row r="279" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B279" s="73"/>
+    <row r="279" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B279" s="74"/>
       <c r="C279" s="33" t="s">
         <v>541</v>
       </c>
@@ -5774,8 +5773,8 @@
       </c>
       <c r="E279" s="11"/>
     </row>
-    <row r="280" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B280" s="73"/>
+    <row r="280" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B280" s="74"/>
       <c r="C280" s="33" t="s">
         <v>542</v>
       </c>
@@ -5784,8 +5783,8 @@
       </c>
       <c r="E280" s="11"/>
     </row>
-    <row r="281" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B281" s="73"/>
+    <row r="281" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B281" s="74"/>
       <c r="C281" s="33" t="s">
         <v>544</v>
       </c>
@@ -5794,8 +5793,8 @@
       </c>
       <c r="E281" s="11"/>
     </row>
-    <row r="282" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B282" s="73"/>
+    <row r="282" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B282" s="74"/>
       <c r="C282" s="33" t="s">
         <v>543</v>
       </c>
@@ -5804,8 +5803,8 @@
       </c>
       <c r="E282" s="11"/>
     </row>
-    <row r="283" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B283" s="73"/>
+    <row r="283" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B283" s="74"/>
       <c r="C283" s="33" t="s">
         <v>545</v>
       </c>
@@ -5814,8 +5813,8 @@
       </c>
       <c r="E283" s="11"/>
     </row>
-    <row r="284" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B284" s="73"/>
+    <row r="284" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B284" s="74"/>
       <c r="C284" s="33" t="s">
         <v>627</v>
       </c>
@@ -5824,8 +5823,8 @@
       </c>
       <c r="E284" s="11"/>
     </row>
-    <row r="285" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B285" s="73"/>
+    <row r="285" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B285" s="74"/>
       <c r="C285" s="33" t="s">
         <v>546</v>
       </c>
@@ -5834,8 +5833,8 @@
       </c>
       <c r="E285" s="11"/>
     </row>
-    <row r="286" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B286" s="73"/>
+    <row r="286" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B286" s="74"/>
       <c r="C286" s="33" t="s">
         <v>547</v>
       </c>
@@ -5844,8 +5843,8 @@
       </c>
       <c r="E286" s="11"/>
     </row>
-    <row r="287" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B287" s="73"/>
+    <row r="287" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B287" s="74"/>
       <c r="C287" s="33" t="s">
         <v>548</v>
       </c>
@@ -5854,8 +5853,8 @@
       </c>
       <c r="E287" s="11"/>
     </row>
-    <row r="288" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B288" s="73"/>
+    <row r="288" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B288" s="74"/>
       <c r="C288" s="33" t="s">
         <v>549</v>
       </c>
@@ -5864,8 +5863,8 @@
       </c>
       <c r="E288" s="11"/>
     </row>
-    <row r="289" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B289" s="73"/>
+    <row r="289" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B289" s="74"/>
       <c r="C289" s="33" t="s">
         <v>550</v>
       </c>
@@ -5874,8 +5873,8 @@
       </c>
       <c r="E289" s="11"/>
     </row>
-    <row r="290" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B290" s="73"/>
+    <row r="290" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B290" s="74"/>
       <c r="C290" s="33" t="s">
         <v>551</v>
       </c>
@@ -5884,8 +5883,8 @@
       </c>
       <c r="E290" s="11"/>
     </row>
-    <row r="291" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B291" s="73"/>
+    <row r="291" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B291" s="74"/>
       <c r="C291" s="33" t="s">
         <v>552</v>
       </c>
@@ -5894,8 +5893,8 @@
       </c>
       <c r="E291" s="11"/>
     </row>
-    <row r="292" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B292" s="73"/>
+    <row r="292" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B292" s="74"/>
       <c r="C292" s="33" t="s">
         <v>553</v>
       </c>
@@ -5904,8 +5903,8 @@
       </c>
       <c r="E292" s="11"/>
     </row>
-    <row r="293" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B293" s="73"/>
+    <row r="293" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B293" s="74"/>
       <c r="C293" s="33" t="s">
         <v>554</v>
       </c>
@@ -5914,8 +5913,8 @@
       </c>
       <c r="E293" s="11"/>
     </row>
-    <row r="294" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B294" s="73"/>
+    <row r="294" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B294" s="74"/>
       <c r="C294" s="33" t="s">
         <v>555</v>
       </c>
@@ -5924,8 +5923,8 @@
       </c>
       <c r="E294" s="11"/>
     </row>
-    <row r="295" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B295" s="73"/>
+    <row r="295" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B295" s="74"/>
       <c r="C295" s="33" t="s">
         <v>556</v>
       </c>
@@ -5934,8 +5933,8 @@
       </c>
       <c r="E295" s="11"/>
     </row>
-    <row r="296" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B296" s="73"/>
+    <row r="296" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B296" s="74"/>
       <c r="C296" s="33" t="s">
         <v>607</v>
       </c>
@@ -5944,8 +5943,8 @@
       </c>
       <c r="E296" s="11"/>
     </row>
-    <row r="297" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B297" s="73"/>
+    <row r="297" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B297" s="74"/>
       <c r="C297" s="33" t="s">
         <v>557</v>
       </c>
@@ -5954,8 +5953,8 @@
       </c>
       <c r="E297" s="11"/>
     </row>
-    <row r="298" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B298" s="73"/>
+    <row r="298" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B298" s="74"/>
       <c r="C298" s="33" t="s">
         <v>560</v>
       </c>
@@ -5964,8 +5963,8 @@
       </c>
       <c r="E298" s="11"/>
     </row>
-    <row r="299" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B299" s="73"/>
+    <row r="299" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B299" s="74"/>
       <c r="C299" s="33" t="s">
         <v>558</v>
       </c>
@@ -5974,8 +5973,8 @@
       </c>
       <c r="E299" s="11"/>
     </row>
-    <row r="300" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B300" s="73"/>
+    <row r="300" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B300" s="74"/>
       <c r="C300" s="33" t="s">
         <v>562</v>
       </c>
@@ -5984,8 +5983,8 @@
       </c>
       <c r="E300" s="11"/>
     </row>
-    <row r="301" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B301" s="73"/>
+    <row r="301" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B301" s="74"/>
       <c r="C301" s="40" t="s">
         <v>559</v>
       </c>
@@ -5994,8 +5993,8 @@
       </c>
       <c r="E301" s="11"/>
     </row>
-    <row r="302" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B302" s="73"/>
+    <row r="302" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B302" s="74"/>
       <c r="C302" s="11" t="s">
         <v>605</v>
       </c>
@@ -6004,18 +6003,18 @@
       </c>
       <c r="E302" s="11"/>
     </row>
-    <row r="303" spans="2:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B303" s="73"/>
-      <c r="C303" s="60" t="s">
+    <row r="303" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B303" s="74"/>
+      <c r="C303" s="58" t="s">
         <v>122</v>
       </c>
-      <c r="D303" s="61" t="s">
+      <c r="D303" s="59" t="s">
         <v>247</v>
       </c>
       <c r="E303" s="11"/>
     </row>
-    <row r="304" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B304" s="73"/>
+    <row r="304" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B304" s="74"/>
       <c r="C304" s="16" t="s">
         <v>123</v>
       </c>
@@ -6024,8 +6023,8 @@
       </c>
       <c r="E304" s="11"/>
     </row>
-    <row r="305" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B305" s="73"/>
+    <row r="305" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B305" s="74"/>
       <c r="C305" s="16" t="s">
         <v>124</v>
       </c>
@@ -6034,8 +6033,8 @@
       </c>
       <c r="E305" s="11"/>
     </row>
-    <row r="306" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B306" s="73"/>
+    <row r="306" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B306" s="74"/>
       <c r="C306" s="16" t="s">
         <v>125</v>
       </c>
@@ -6044,8 +6043,8 @@
       </c>
       <c r="E306" s="11"/>
     </row>
-    <row r="307" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B307" s="73"/>
+    <row r="307" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B307" s="74"/>
       <c r="C307" s="16" t="s">
         <v>126</v>
       </c>
@@ -6054,8 +6053,8 @@
       </c>
       <c r="E307" s="11"/>
     </row>
-    <row r="308" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B308" s="73"/>
+    <row r="308" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B308" s="74"/>
       <c r="C308" s="16" t="s">
         <v>128</v>
       </c>
@@ -6064,8 +6063,8 @@
       </c>
       <c r="E308" s="11"/>
     </row>
-    <row r="309" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B309" s="73"/>
+    <row r="309" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B309" s="74"/>
       <c r="C309" s="11" t="s">
         <v>127</v>
       </c>
@@ -6074,8 +6073,8 @@
       </c>
       <c r="E309" s="11"/>
     </row>
-    <row r="310" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B310" s="73"/>
+    <row r="310" spans="2:5" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B310" s="74"/>
       <c r="C310" s="17" t="s">
         <v>129</v>
       </c>
@@ -6084,8 +6083,8 @@
       </c>
       <c r="E310" s="37"/>
     </row>
-    <row r="311" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B311" s="72" t="s">
+    <row r="311" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B311" s="86" t="s">
         <v>349</v>
       </c>
       <c r="C311" s="3" t="s">
@@ -6096,8 +6095,8 @@
       </c>
       <c r="E311" s="4"/>
     </row>
-    <row r="312" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B312" s="73"/>
+    <row r="312" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B312" s="74"/>
       <c r="C312" s="5" t="s">
         <v>10</v>
       </c>
@@ -6106,8 +6105,8 @@
       </c>
       <c r="E312" s="6"/>
     </row>
-    <row r="313" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B313" s="73"/>
+    <row r="313" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B313" s="74"/>
       <c r="C313" s="5" t="s">
         <v>1</v>
       </c>
@@ -6116,8 +6115,8 @@
       </c>
       <c r="E313" s="6"/>
     </row>
-    <row r="314" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B314" s="73"/>
+    <row r="314" spans="2:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B314" s="74"/>
       <c r="C314" s="5" t="s">
         <v>13</v>
       </c>
@@ -6126,8 +6125,8 @@
       </c>
       <c r="E314" s="6"/>
     </row>
-    <row r="315" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B315" s="74"/>
+    <row r="315" spans="2:5" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B315" s="77"/>
       <c r="C315" s="9" t="s">
         <v>12</v>
       </c>
@@ -6138,6 +6137,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E155:E187"/>
+    <mergeCell ref="B155:B187"/>
+    <mergeCell ref="B311:B315"/>
+    <mergeCell ref="B197:B310"/>
+    <mergeCell ref="B192:B196"/>
+    <mergeCell ref="B188:B191"/>
     <mergeCell ref="B100:B154"/>
     <mergeCell ref="E7:E13"/>
     <mergeCell ref="B88:B90"/>
@@ -6147,17 +6152,13 @@
     <mergeCell ref="E88:E90"/>
     <mergeCell ref="E27:E41"/>
     <mergeCell ref="E51:E75"/>
-    <mergeCell ref="E155:E187"/>
-    <mergeCell ref="B155:B187"/>
-    <mergeCell ref="B311:B315"/>
-    <mergeCell ref="B197:B310"/>
-    <mergeCell ref="B192:B196"/>
-    <mergeCell ref="B188:B191"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="54" fitToHeight="6" orientation="portrait" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
+  <headerFooter alignWithMargins="0">
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Tahoma"&amp;9&amp;KCF022B C2 - Eingeschränkte Verwendung</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -6168,15 +6169,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004F7AABC398522B40A32DAEEC36E85685" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fcd56fbdc9ca50fa66f2b7c9cf7a93ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="246f02dd96380beb4f7cdcce14d77fd6">
     <xsd:element name="properties">
@@ -6225,6 +6217,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9B769F7-9146-41B9-ADB1-A4583690659C}">
   <ds:schemaRefs>
@@ -6241,14 +6242,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{083AA8F9-0094-42DD-9088-30A041B6BBAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28CD8B8F-7010-4154-9283-2E108768C2EF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6261,4 +6254,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{083AA8F9-0094-42DD-9088-30A041B6BBAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>